<commit_message>
excel update work, pt i
</commit_message>
<xml_diff>
--- a/new.xlsx
+++ b/new.xlsx
@@ -21,7 +21,7 @@
     <sheet name="TZs" sheetId="5" r:id="rId11"/>
     <sheet name="SupportLists" sheetId="8" r:id="rId12"/>
   </sheets>
-  <calcPr calcId="191029"/>
+  <calcPr calcId="191029" fullCalcOnLoad="1"/>
   <extLst>
     <ext uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -970,6 +970,9 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision">
+  <numFmts count="1">
+    <numFmt numFmtId="164" formatCode="dd.mm.YYYY"/>
+  </numFmts>
   <fonts count="7">
     <font>
       <name val="Aptos Narrow"/>
@@ -1037,7 +1040,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="12">
+  <cellXfs count="13">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -1052,6 +1055,7 @@
     </xf>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -5368,7 +5372,7 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3">
-  <dimension ref="A1:E88"/>
+  <dimension ref="A1:E156"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A6" sqref="A6"/>
@@ -6994,60 +6998,1352 @@
       </c>
     </row>
     <row r="86" spans="1:5" customFormat="false">
-      <c r="A86">
+      <c r="A86" s="0">
         <f>VLOOKUP(B86,IDs!B:C,2,FALSE)</f>
-        <v>0</v>
-      </c>
-      <c r="B86" t="s">
-        <v>117</v>
-      </c>
-      <c r="C86">
-        <v>28550286</v>
-      </c>
-      <c r="D86" s="5">
-        <v>45539</v>
-      </c>
-      <c r="E86">
-        <f>VLOOKUP(D86,SupportLists!D:E,2,FALSE)</f>
-        <v>1</v>
+        <v/>
+      </c>
+      <c r="B86" s="0" t="str">
+        <v>Garrrfield</v>
+      </c>
+      <c r="C86" s="0">
+        <v>35751242</v>
+      </c>
+      <c r="D86" s="12">
+        <v>45584.0</v>
+      </c>
+      <c r="E86" s="0">
+        <f>A86 &amp; "|" &amp; VLOOKUP(D86,SupportLists!D:E,2,FALSE)</f>
+        <v/>
       </c>
     </row>
     <row r="87" spans="1:5" customFormat="false">
-      <c r="A87" t="str">
+      <c r="A87" s="0">
         <f>VLOOKUP(B87,IDs!B:C,2,FALSE)</f>
-        <v>PVYB6A5F</v>
-      </c>
-      <c r="B87" t="s">
-        <v>130</v>
-      </c>
-      <c r="C87">
-        <v>27048359</v>
-      </c>
-      <c r="D87" s="5">
-        <v>45539</v>
-      </c>
-      <c r="E87">
-        <f>VLOOKUP(D87,SupportLists!D:E,2,FALSE)</f>
-        <v>1</v>
+        <v/>
+      </c>
+      <c r="B87" s="0" t="str">
+        <v>LittleKnights</v>
+      </c>
+      <c r="C87" s="0">
+        <v>55272769</v>
+      </c>
+      <c r="D87" s="12">
+        <v>45584.0</v>
+      </c>
+      <c r="E87" s="0">
+        <f>A87 &amp; "|" &amp; VLOOKUP(D87,SupportLists!D:E,2,FALSE)</f>
+        <v/>
       </c>
     </row>
     <row r="88" spans="1:5" customFormat="false">
-      <c r="A88" t="str">
+      <c r="A88" s="0">
         <f>VLOOKUP(B88,IDs!B:C,2,FALSE)</f>
-        <v>P8W89A5U</v>
-      </c>
-      <c r="B88" t="s">
-        <v>128</v>
-      </c>
-      <c r="C88">
-        <v>26431053</v>
-      </c>
-      <c r="D88" s="5">
-        <v>45539</v>
-      </c>
-      <c r="E88">
-        <f>VLOOKUP(D88,SupportLists!D:E,2,FALSE)</f>
-        <v>1</v>
+        <v/>
+      </c>
+      <c r="B88" s="0" t="str">
+        <v>Xorron</v>
+      </c>
+      <c r="C88" s="0">
+        <v>46884042</v>
+      </c>
+      <c r="D88" s="12">
+        <v>45584.0</v>
+      </c>
+      <c r="E88" s="0">
+        <f>A88 &amp; "|" &amp; VLOOKUP(D88,SupportLists!D:E,2,FALSE)</f>
+        <v/>
+      </c>
+    </row>
+    <row r="89" spans="1:5" customFormat="false">
+      <c r="A89" s="0">
+        <f>VLOOKUP(B89,IDs!B:C,2,FALSE)</f>
+        <v/>
+      </c>
+      <c r="B89" s="0" t="str">
+        <v>Kyredneck30</v>
+      </c>
+      <c r="C89" s="0">
+        <v>45717123</v>
+      </c>
+      <c r="D89" s="12">
+        <v>45584.0</v>
+      </c>
+      <c r="E89" s="0">
+        <f>A89 &amp; "|" &amp; VLOOKUP(D89,SupportLists!D:E,2,FALSE)</f>
+        <v/>
+      </c>
+    </row>
+    <row r="90" spans="1:5" customFormat="false">
+      <c r="A90" s="0">
+        <f>VLOOKUP(B90,IDs!B:C,2,FALSE)</f>
+        <v/>
+      </c>
+      <c r="B90" s="0" t="str">
+        <v>SoulKnightSK</v>
+      </c>
+      <c r="C90" s="0">
+        <v>68482687</v>
+      </c>
+      <c r="D90" s="12">
+        <v>45584.0</v>
+      </c>
+      <c r="E90" s="0">
+        <f>A90 &amp; "|" &amp; VLOOKUP(D90,SupportLists!D:E,2,FALSE)</f>
+        <v/>
+      </c>
+    </row>
+    <row r="91" spans="1:5" customFormat="false">
+      <c r="A91" s="0">
+        <f>VLOOKUP(B91,IDs!B:C,2,FALSE)</f>
+        <v/>
+      </c>
+      <c r="B91" s="0" t="str">
+        <v>Schneeman</v>
+      </c>
+      <c r="C91" s="0">
+        <v>52625609</v>
+      </c>
+      <c r="D91" s="12">
+        <v>45584.0</v>
+      </c>
+      <c r="E91" s="0">
+        <f>A91 &amp; "|" &amp; VLOOKUP(D91,SupportLists!D:E,2,FALSE)</f>
+        <v/>
+      </c>
+    </row>
+    <row r="92" spans="1:5" customFormat="false">
+      <c r="A92" s="0">
+        <f>VLOOKUP(B92,IDs!B:C,2,FALSE)</f>
+        <v/>
+      </c>
+      <c r="B92" s="0" t="str">
+        <v>Letsii</v>
+      </c>
+      <c r="C92" s="0">
+        <v>46742185</v>
+      </c>
+      <c r="D92" s="12">
+        <v>45584.0</v>
+      </c>
+      <c r="E92" s="0">
+        <f>A92 &amp; "|" &amp; VLOOKUP(D92,SupportLists!D:E,2,FALSE)</f>
+        <v/>
+      </c>
+    </row>
+    <row r="93" spans="1:5" customFormat="false">
+      <c r="A93" s="0">
+        <f>VLOOKUP(B93,IDs!B:C,2,FALSE)</f>
+        <v/>
+      </c>
+      <c r="B93" s="0" t="str">
+        <v>Daeloan</v>
+      </c>
+      <c r="C93" s="0">
+        <v>78221959</v>
+      </c>
+      <c r="D93" s="12">
+        <v>45584.0</v>
+      </c>
+      <c r="E93" s="0">
+        <f>A93 &amp; "|" &amp; VLOOKUP(D93,SupportLists!D:E,2,FALSE)</f>
+        <v/>
+      </c>
+    </row>
+    <row r="94" spans="1:5" customFormat="false">
+      <c r="A94" s="0">
+        <f>VLOOKUP(B94,IDs!B:C,2,FALSE)</f>
+        <v/>
+      </c>
+      <c r="B94" s="0" t="str">
+        <v>finanzamtt</v>
+      </c>
+      <c r="C94" s="0">
+        <v>60805758</v>
+      </c>
+      <c r="D94" s="12">
+        <v>45584.0</v>
+      </c>
+      <c r="E94" s="0">
+        <f>A94 &amp; "|" &amp; VLOOKUP(D94,SupportLists!D:E,2,FALSE)</f>
+        <v/>
+      </c>
+    </row>
+    <row r="95" spans="1:5" customFormat="false">
+      <c r="A95" s="0">
+        <f>VLOOKUP(B95,IDs!B:C,2,FALSE)</f>
+        <v/>
+      </c>
+      <c r="B95" s="0" t="str">
+        <v>Sevenupurs</v>
+      </c>
+      <c r="C95" s="0">
+        <v>60450559</v>
+      </c>
+      <c r="D95" s="12">
+        <v>45584.0</v>
+      </c>
+      <c r="E95" s="0">
+        <f>A95 &amp; "|" &amp; VLOOKUP(D95,SupportLists!D:E,2,FALSE)</f>
+        <v/>
+      </c>
+    </row>
+    <row r="96" spans="1:5" customFormat="false">
+      <c r="A96" s="0">
+        <f>VLOOKUP(B96,IDs!B:C,2,FALSE)</f>
+        <v/>
+      </c>
+      <c r="B96" s="0" t="str">
+        <v>ShaRopi69</v>
+      </c>
+      <c r="C96" s="0">
+        <v>55798182</v>
+      </c>
+      <c r="D96" s="12">
+        <v>45584.0</v>
+      </c>
+      <c r="E96" s="0">
+        <f>A96 &amp; "|" &amp; VLOOKUP(D96,SupportLists!D:E,2,FALSE)</f>
+        <v/>
+      </c>
+    </row>
+    <row r="97" spans="1:5" customFormat="false">
+      <c r="A97" s="0">
+        <f>VLOOKUP(B97,IDs!B:C,2,FALSE)</f>
+        <v/>
+      </c>
+      <c r="B97" s="0" t="str">
+        <v>MR.Grinch</v>
+      </c>
+      <c r="C97" s="0">
+        <v>54016906</v>
+      </c>
+      <c r="D97" s="12">
+        <v>45584.0</v>
+      </c>
+      <c r="E97" s="0">
+        <f>A97 &amp; "|" &amp; VLOOKUP(D97,SupportLists!D:E,2,FALSE)</f>
+        <v/>
+      </c>
+    </row>
+    <row r="98" spans="1:5" customFormat="false">
+      <c r="A98" s="0">
+        <f>VLOOKUP(B98,IDs!B:C,2,FALSE)</f>
+        <v/>
+      </c>
+      <c r="B98" s="0" t="str">
+        <v>xljhx31</v>
+      </c>
+      <c r="C98" s="0">
+        <v>51309966</v>
+      </c>
+      <c r="D98" s="12">
+        <v>45584.0</v>
+      </c>
+      <c r="E98" s="0">
+        <f>A98 &amp; "|" &amp; VLOOKUP(D98,SupportLists!D:E,2,FALSE)</f>
+        <v/>
+      </c>
+    </row>
+    <row r="99" spans="1:5" customFormat="false">
+      <c r="A99" s="0">
+        <f>VLOOKUP(B99,IDs!B:C,2,FALSE)</f>
+        <v/>
+      </c>
+      <c r="B99" s="0" t="str">
+        <v>RJShuda</v>
+      </c>
+      <c r="C99" s="0">
+        <v>44955250</v>
+      </c>
+      <c r="D99" s="12">
+        <v>45584.0</v>
+      </c>
+      <c r="E99" s="0">
+        <f>A99 &amp; "|" &amp; VLOOKUP(D99,SupportLists!D:E,2,FALSE)</f>
+        <v/>
+      </c>
+    </row>
+    <row r="100" spans="1:5" customFormat="false">
+      <c r="A100" s="0">
+        <f>VLOOKUP(B100,IDs!B:C,2,FALSE)</f>
+        <v/>
+      </c>
+      <c r="B100" s="0" t="str">
+        <v>Evita.Q</v>
+      </c>
+      <c r="C100" s="0">
+        <v>42177593</v>
+      </c>
+      <c r="D100" s="12">
+        <v>45584.0</v>
+      </c>
+      <c r="E100" s="0">
+        <f>A100 &amp; "|" &amp; VLOOKUP(D100,SupportLists!D:E,2,FALSE)</f>
+        <v/>
+      </c>
+    </row>
+    <row r="101" spans="1:5" customFormat="false">
+      <c r="A101" s="0">
+        <f>VLOOKUP(B101,IDs!B:C,2,FALSE)</f>
+        <v/>
+      </c>
+      <c r="B101" s="0" t="str">
+        <v>DangerMouse</v>
+      </c>
+      <c r="C101" s="0">
+        <v>41222530</v>
+      </c>
+      <c r="D101" s="12">
+        <v>45584.0</v>
+      </c>
+      <c r="E101" s="0">
+        <f>A101 &amp; "|" &amp; VLOOKUP(D101,SupportLists!D:E,2,FALSE)</f>
+        <v/>
+      </c>
+    </row>
+    <row r="102" spans="1:5" customFormat="false">
+      <c r="A102" s="0">
+        <f>VLOOKUP(B102,IDs!B:C,2,FALSE)</f>
+        <v/>
+      </c>
+      <c r="B102" s="0" t="str">
+        <v>dragSD</v>
+      </c>
+      <c r="C102" s="0">
+        <v>40263474</v>
+      </c>
+      <c r="D102" s="12">
+        <v>45584.0</v>
+      </c>
+      <c r="E102" s="0">
+        <f>A102 &amp; "|" &amp; VLOOKUP(D102,SupportLists!D:E,2,FALSE)</f>
+        <v/>
+      </c>
+    </row>
+    <row r="103" spans="1:5" customFormat="false">
+      <c r="A103" s="0">
+        <f>VLOOKUP(B103,IDs!B:C,2,FALSE)</f>
+        <v/>
+      </c>
+      <c r="B103" s="0" t="str">
+        <v>Goldvale</v>
+      </c>
+      <c r="C103" s="0">
+        <v>36918040</v>
+      </c>
+      <c r="D103" s="12">
+        <v>45584.0</v>
+      </c>
+      <c r="E103" s="0">
+        <f>A103 &amp; "|" &amp; VLOOKUP(D103,SupportLists!D:E,2,FALSE)</f>
+        <v/>
+      </c>
+    </row>
+    <row r="104" spans="1:5" customFormat="false">
+      <c r="A104" s="0">
+        <f>VLOOKUP(B104,IDs!B:C,2,FALSE)</f>
+        <v/>
+      </c>
+      <c r="B104" s="0" t="str">
+        <v>TrebleMaker</v>
+      </c>
+      <c r="C104" s="0">
+        <v>36297525</v>
+      </c>
+      <c r="D104" s="12">
+        <v>45584.0</v>
+      </c>
+      <c r="E104" s="0">
+        <f>A104 &amp; "|" &amp; VLOOKUP(D104,SupportLists!D:E,2,FALSE)</f>
+        <v/>
+      </c>
+    </row>
+    <row r="105" spans="1:5" customFormat="false">
+      <c r="A105" s="0">
+        <f>VLOOKUP(B105,IDs!B:C,2,FALSE)</f>
+        <v/>
+      </c>
+      <c r="B105" s="0" t="str">
+        <v>KingLiz</v>
+      </c>
+      <c r="C105" s="0">
+        <v>35924718</v>
+      </c>
+      <c r="D105" s="12">
+        <v>45584.0</v>
+      </c>
+      <c r="E105" s="0">
+        <f>A105 &amp; "|" &amp; VLOOKUP(D105,SupportLists!D:E,2,FALSE)</f>
+        <v/>
+      </c>
+    </row>
+    <row r="106" spans="1:5" customFormat="false">
+      <c r="A106" s="0">
+        <f>VLOOKUP(B106,IDs!B:C,2,FALSE)</f>
+        <v/>
+      </c>
+      <c r="B106" s="0" t="str">
+        <v>mido009</v>
+      </c>
+      <c r="C106" s="0">
+        <v>41196673</v>
+      </c>
+      <c r="D106" s="12">
+        <v>45584.0</v>
+      </c>
+      <c r="E106" s="0">
+        <f>A106 &amp; "|" &amp; VLOOKUP(D106,SupportLists!D:E,2,FALSE)</f>
+        <v/>
+      </c>
+    </row>
+    <row r="107" spans="1:5" customFormat="false">
+      <c r="A107" s="0">
+        <f>VLOOKUP(B107,IDs!B:C,2,FALSE)</f>
+        <v/>
+      </c>
+      <c r="B107" s="0" t="str">
+        <v>Maria4612</v>
+      </c>
+      <c r="C107" s="0">
+        <v>38974543</v>
+      </c>
+      <c r="D107" s="12">
+        <v>45584.0</v>
+      </c>
+      <c r="E107" s="0">
+        <f>A107 &amp; "|" &amp; VLOOKUP(D107,SupportLists!D:E,2,FALSE)</f>
+        <v/>
+      </c>
+    </row>
+    <row r="108" spans="1:5" customFormat="false">
+      <c r="A108" s="0">
+        <f>VLOOKUP(B108,IDs!B:C,2,FALSE)</f>
+        <v/>
+      </c>
+      <c r="B108" s="0" t="str">
+        <v>RaquelsHero</v>
+      </c>
+      <c r="C108" s="0">
+        <v>36445384</v>
+      </c>
+      <c r="D108" s="12">
+        <v>45584.0</v>
+      </c>
+      <c r="E108" s="0">
+        <f>A108 &amp; "|" &amp; VLOOKUP(D108,SupportLists!D:E,2,FALSE)</f>
+        <v/>
+      </c>
+    </row>
+    <row r="109" spans="1:5" customFormat="false">
+      <c r="A109" s="0">
+        <f>VLOOKUP(B109,IDs!B:C,2,FALSE)</f>
+        <v/>
+      </c>
+      <c r="B109" s="0" t="str">
+        <v>I am Groot</v>
+      </c>
+      <c r="C109" s="0">
+        <v>35973077</v>
+      </c>
+      <c r="D109" s="12">
+        <v>45584.0</v>
+      </c>
+      <c r="E109" s="0">
+        <f>A109 &amp; "|" &amp; VLOOKUP(D109,SupportLists!D:E,2,FALSE)</f>
+        <v/>
+      </c>
+    </row>
+    <row r="110" spans="1:5" customFormat="false">
+      <c r="A110" s="0">
+        <f>VLOOKUP(B110,IDs!B:C,2,FALSE)</f>
+        <v/>
+      </c>
+      <c r="B110" s="0" t="str">
+        <v>VON</v>
+      </c>
+      <c r="C110" s="0">
+        <v>35437997</v>
+      </c>
+      <c r="D110" s="12">
+        <v>45584.0</v>
+      </c>
+      <c r="E110" s="0">
+        <f>A110 &amp; "|" &amp; VLOOKUP(D110,SupportLists!D:E,2,FALSE)</f>
+        <v/>
+      </c>
+    </row>
+    <row r="111" spans="1:5" customFormat="false">
+      <c r="A111" s="0">
+        <f>VLOOKUP(B111,IDs!B:C,2,FALSE)</f>
+        <v/>
+      </c>
+      <c r="B111" s="0" t="str">
+        <v>Alecks_</v>
+      </c>
+      <c r="C111" s="0">
+        <v>70136709</v>
+      </c>
+      <c r="D111" s="12">
+        <v>45584.0</v>
+      </c>
+      <c r="E111" s="0">
+        <f>A111 &amp; "|" &amp; VLOOKUP(D111,SupportLists!D:E,2,FALSE)</f>
+        <v/>
+      </c>
+    </row>
+    <row r="112" spans="1:5" customFormat="false">
+      <c r="A112" s="0">
+        <f>VLOOKUP(B112,IDs!B:C,2,FALSE)</f>
+        <v/>
+      </c>
+      <c r="B112" s="0" t="str">
+        <v>itaca90909090</v>
+      </c>
+      <c r="C112" s="0">
+        <v>54132050</v>
+      </c>
+      <c r="D112" s="12">
+        <v>45584.0</v>
+      </c>
+      <c r="E112" s="0">
+        <f>A112 &amp; "|" &amp; VLOOKUP(D112,SupportLists!D:E,2,FALSE)</f>
+        <v/>
+      </c>
+    </row>
+    <row r="113" spans="1:5" customFormat="false">
+      <c r="A113" s="0">
+        <f>VLOOKUP(B113,IDs!B:C,2,FALSE)</f>
+        <v/>
+      </c>
+      <c r="B113" s="0" t="str">
+        <v>Nefi85</v>
+      </c>
+      <c r="C113" s="0">
+        <v>44311802</v>
+      </c>
+      <c r="D113" s="12">
+        <v>45584.0</v>
+      </c>
+      <c r="E113" s="0">
+        <f>A113 &amp; "|" &amp; VLOOKUP(D113,SupportLists!D:E,2,FALSE)</f>
+        <v/>
+      </c>
+    </row>
+    <row r="114" spans="1:5" customFormat="false">
+      <c r="A114" s="0">
+        <f>VLOOKUP(B114,IDs!B:C,2,FALSE)</f>
+        <v/>
+      </c>
+      <c r="B114" s="0" t="str">
+        <v>Permobil</v>
+      </c>
+      <c r="C114" s="0">
+        <v>42022280</v>
+      </c>
+      <c r="D114" s="12">
+        <v>45584.0</v>
+      </c>
+      <c r="E114" s="0">
+        <f>A114 &amp; "|" &amp; VLOOKUP(D114,SupportLists!D:E,2,FALSE)</f>
+        <v/>
+      </c>
+    </row>
+    <row r="115" spans="1:5" customFormat="false">
+      <c r="A115" s="0">
+        <f>VLOOKUP(B115,IDs!B:C,2,FALSE)</f>
+        <v/>
+      </c>
+      <c r="B115" s="0" t="str">
+        <v>Niimphy</v>
+      </c>
+      <c r="C115" s="0">
+        <v>35999933</v>
+      </c>
+      <c r="D115" s="12">
+        <v>45584.0</v>
+      </c>
+      <c r="E115" s="0">
+        <f>A115 &amp; "|" &amp; VLOOKUP(D115,SupportLists!D:E,2,FALSE)</f>
+        <v/>
+      </c>
+    </row>
+    <row r="116" spans="1:5" customFormat="false">
+      <c r="A116" s="0">
+        <f>VLOOKUP(B116,IDs!B:C,2,FALSE)</f>
+        <v/>
+      </c>
+      <c r="B116" s="0" t="str">
+        <v>Daut</v>
+      </c>
+      <c r="C116" s="0">
+        <v>50140283</v>
+      </c>
+      <c r="D116" s="12">
+        <v>45584.0</v>
+      </c>
+      <c r="E116" s="0">
+        <f>A116 &amp; "|" &amp; VLOOKUP(D116,SupportLists!D:E,2,FALSE)</f>
+        <v/>
+      </c>
+    </row>
+    <row r="117" spans="1:5" customFormat="false">
+      <c r="A117" s="0">
+        <f>VLOOKUP(B117,IDs!B:C,2,FALSE)</f>
+        <v/>
+      </c>
+      <c r="B117" s="0" t="str">
+        <v>ZeroX_47</v>
+      </c>
+      <c r="C117" s="0">
+        <v>42208168</v>
+      </c>
+      <c r="D117" s="12">
+        <v>45584.0</v>
+      </c>
+      <c r="E117" s="0">
+        <f>A117 &amp; "|" &amp; VLOOKUP(D117,SupportLists!D:E,2,FALSE)</f>
+        <v/>
+      </c>
+    </row>
+    <row r="118" spans="1:5" customFormat="false">
+      <c r="A118" s="0">
+        <f>VLOOKUP(B118,IDs!B:C,2,FALSE)</f>
+        <v/>
+      </c>
+      <c r="B118" s="0" t="str">
+        <v>Schockaletta</v>
+      </c>
+      <c r="C118" s="0">
+        <v>36600286</v>
+      </c>
+      <c r="D118" s="12">
+        <v>45584.0</v>
+      </c>
+      <c r="E118" s="0">
+        <f>A118 &amp; "|" &amp; VLOOKUP(D118,SupportLists!D:E,2,FALSE)</f>
+        <v/>
+      </c>
+    </row>
+    <row r="119" spans="1:5" customFormat="false">
+      <c r="A119" s="0">
+        <f>VLOOKUP(B119,IDs!B:C,2,FALSE)</f>
+        <v/>
+      </c>
+      <c r="B119" s="0" t="str">
+        <v>LESINVINCIBLES</v>
+      </c>
+      <c r="C119" s="0">
+        <v>31135467</v>
+      </c>
+      <c r="D119" s="12">
+        <v>45584.0</v>
+      </c>
+      <c r="E119" s="0">
+        <f>A119 &amp; "|" &amp; VLOOKUP(D119,SupportLists!D:E,2,FALSE)</f>
+        <v/>
+      </c>
+    </row>
+    <row r="120" spans="1:5" customFormat="false">
+      <c r="A120" s="0">
+        <f>VLOOKUP(B120,IDs!B:C,2,FALSE)</f>
+        <v/>
+      </c>
+      <c r="B120" s="0" t="str">
+        <v>POLAR-BEAR</v>
+      </c>
+      <c r="C120" s="0">
+        <v>61121304</v>
+      </c>
+      <c r="D120" s="12">
+        <v>45584.0</v>
+      </c>
+      <c r="E120" s="0">
+        <f>A120 &amp; "|" &amp; VLOOKUP(D120,SupportLists!D:E,2,FALSE)</f>
+        <v/>
+      </c>
+    </row>
+    <row r="121" spans="1:5" customFormat="false">
+      <c r="A121" s="0">
+        <f>VLOOKUP(B121,IDs!B:C,2,FALSE)</f>
+        <v/>
+      </c>
+      <c r="B121" s="0" t="str">
+        <v>ShyDust</v>
+      </c>
+      <c r="C121" s="0">
+        <v>60245369</v>
+      </c>
+      <c r="D121" s="12">
+        <v>45584.0</v>
+      </c>
+      <c r="E121" s="0">
+        <f>A121 &amp; "|" &amp; VLOOKUP(D121,SupportLists!D:E,2,FALSE)</f>
+        <v/>
+      </c>
+    </row>
+    <row r="122" spans="1:5" customFormat="false">
+      <c r="A122" s="0">
+        <f>VLOOKUP(B122,IDs!B:C,2,FALSE)</f>
+        <v/>
+      </c>
+      <c r="B122" s="0" t="str">
+        <v>SKIF3006</v>
+      </c>
+      <c r="C122" s="0">
+        <v>49544841</v>
+      </c>
+      <c r="D122" s="12">
+        <v>45584.0</v>
+      </c>
+      <c r="E122" s="0">
+        <f>A122 &amp; "|" &amp; VLOOKUP(D122,SupportLists!D:E,2,FALSE)</f>
+        <v/>
+      </c>
+    </row>
+    <row r="123" spans="1:5" customFormat="false">
+      <c r="A123" s="0">
+        <f>VLOOKUP(B123,IDs!B:C,2,FALSE)</f>
+        <v/>
+      </c>
+      <c r="B123" s="0" t="str">
+        <v>NOAH</v>
+      </c>
+      <c r="C123" s="0">
+        <v>47409011</v>
+      </c>
+      <c r="D123" s="12">
+        <v>45584.0</v>
+      </c>
+      <c r="E123" s="0">
+        <f>A123 &amp; "|" &amp; VLOOKUP(D123,SupportLists!D:E,2,FALSE)</f>
+        <v/>
+      </c>
+    </row>
+    <row r="124" spans="1:5" customFormat="false">
+      <c r="A124" s="0">
+        <f>VLOOKUP(B124,IDs!B:C,2,FALSE)</f>
+        <v/>
+      </c>
+      <c r="B124" s="0" t="str">
+        <v>Kevo1707</v>
+      </c>
+      <c r="C124" s="0">
+        <v>47285414</v>
+      </c>
+      <c r="D124" s="12">
+        <v>45584.0</v>
+      </c>
+      <c r="E124" s="0">
+        <f>A124 &amp; "|" &amp; VLOOKUP(D124,SupportLists!D:E,2,FALSE)</f>
+        <v/>
+      </c>
+    </row>
+    <row r="125" spans="1:5" customFormat="false">
+      <c r="A125" s="0">
+        <f>VLOOKUP(B125,IDs!B:C,2,FALSE)</f>
+        <v/>
+      </c>
+      <c r="B125" s="0" t="str">
+        <v>Grizzly</v>
+      </c>
+      <c r="C125" s="0">
+        <v>45802878</v>
+      </c>
+      <c r="D125" s="12">
+        <v>45584.0</v>
+      </c>
+      <c r="E125" s="0">
+        <f>A125 &amp; "|" &amp; VLOOKUP(D125,SupportLists!D:E,2,FALSE)</f>
+        <v/>
+      </c>
+    </row>
+    <row r="126" spans="1:5" customFormat="false">
+      <c r="A126" s="0">
+        <f>VLOOKUP(B126,IDs!B:C,2,FALSE)</f>
+        <v/>
+      </c>
+      <c r="B126" s="0" t="str">
+        <v>GhostSlayer</v>
+      </c>
+      <c r="C126" s="0">
+        <v>47375039</v>
+      </c>
+      <c r="D126" s="12">
+        <v>45584.0</v>
+      </c>
+      <c r="E126" s="0">
+        <f>A126 &amp; "|" &amp; VLOOKUP(D126,SupportLists!D:E,2,FALSE)</f>
+        <v/>
+      </c>
+    </row>
+    <row r="127" spans="1:5" customFormat="false">
+      <c r="A127" s="0">
+        <f>VLOOKUP(B127,IDs!B:C,2,FALSE)</f>
+        <v/>
+      </c>
+      <c r="B127" s="0" t="str">
+        <v>Busijay</v>
+      </c>
+      <c r="C127" s="0">
+        <v>45909959</v>
+      </c>
+      <c r="D127" s="12">
+        <v>45584.0</v>
+      </c>
+      <c r="E127" s="0">
+        <f>A127 &amp; "|" &amp; VLOOKUP(D127,SupportLists!D:E,2,FALSE)</f>
+        <v/>
+      </c>
+    </row>
+    <row r="128" spans="1:5" customFormat="false">
+      <c r="A128" s="0">
+        <f>VLOOKUP(B128,IDs!B:C,2,FALSE)</f>
+        <v/>
+      </c>
+      <c r="B128" s="0" t="str">
+        <v>Stefan333</v>
+      </c>
+      <c r="C128" s="0">
+        <v>45637522</v>
+      </c>
+      <c r="D128" s="12">
+        <v>45584.0</v>
+      </c>
+      <c r="E128" s="0">
+        <f>A128 &amp; "|" &amp; VLOOKUP(D128,SupportLists!D:E,2,FALSE)</f>
+        <v/>
+      </c>
+    </row>
+    <row r="129" spans="1:5" customFormat="false">
+      <c r="A129" s="0">
+        <f>VLOOKUP(B129,IDs!B:C,2,FALSE)</f>
+        <v/>
+      </c>
+      <c r="B129" s="0" t="str">
+        <v>CharLee</v>
+      </c>
+      <c r="C129" s="0">
+        <v>44549137</v>
+      </c>
+      <c r="D129" s="12">
+        <v>45584.0</v>
+      </c>
+      <c r="E129" s="0">
+        <f>A129 &amp; "|" &amp; VLOOKUP(D129,SupportLists!D:E,2,FALSE)</f>
+        <v/>
+      </c>
+    </row>
+    <row r="130" spans="1:5" customFormat="false">
+      <c r="A130" s="0">
+        <f>VLOOKUP(B130,IDs!B:C,2,FALSE)</f>
+        <v/>
+      </c>
+      <c r="B130" s="0" t="str">
+        <v>Ruby Sunday</v>
+      </c>
+      <c r="C130" s="0">
+        <v>44237063</v>
+      </c>
+      <c r="D130" s="12">
+        <v>45584.0</v>
+      </c>
+      <c r="E130" s="0">
+        <f>A130 &amp; "|" &amp; VLOOKUP(D130,SupportLists!D:E,2,FALSE)</f>
+        <v/>
+      </c>
+    </row>
+    <row r="131" spans="1:5" customFormat="false">
+      <c r="A131" s="0">
+        <f>VLOOKUP(B131,IDs!B:C,2,FALSE)</f>
+        <v/>
+      </c>
+      <c r="B131" s="0" t="str">
+        <v>RockerFoo</v>
+      </c>
+      <c r="C131" s="0">
+        <v>43864931</v>
+      </c>
+      <c r="D131" s="12">
+        <v>45584.0</v>
+      </c>
+      <c r="E131" s="0">
+        <f>A131 &amp; "|" &amp; VLOOKUP(D131,SupportLists!D:E,2,FALSE)</f>
+        <v/>
+      </c>
+    </row>
+    <row r="132" spans="1:5" customFormat="false">
+      <c r="A132" s="0">
+        <f>VLOOKUP(B132,IDs!B:C,2,FALSE)</f>
+        <v/>
+      </c>
+      <c r="B132" s="0" t="str">
+        <v>Hallen98</v>
+      </c>
+      <c r="C132" s="0">
+        <v>43038395</v>
+      </c>
+      <c r="D132" s="12">
+        <v>45584.0</v>
+      </c>
+      <c r="E132" s="0">
+        <f>A132 &amp; "|" &amp; VLOOKUP(D132,SupportLists!D:E,2,FALSE)</f>
+        <v/>
+      </c>
+    </row>
+    <row r="133" spans="1:5" customFormat="false">
+      <c r="A133" s="0">
+        <f>VLOOKUP(B133,IDs!B:C,2,FALSE)</f>
+        <v/>
+      </c>
+      <c r="B133" s="0" t="str">
+        <v>The RoastPotato</v>
+      </c>
+      <c r="C133" s="0">
+        <v>41356377</v>
+      </c>
+      <c r="D133" s="12">
+        <v>45584.0</v>
+      </c>
+      <c r="E133" s="0">
+        <f>A133 &amp; "|" &amp; VLOOKUP(D133,SupportLists!D:E,2,FALSE)</f>
+        <v/>
+      </c>
+    </row>
+    <row r="134" spans="1:5" customFormat="false">
+      <c r="A134" s="0">
+        <f>VLOOKUP(B134,IDs!B:C,2,FALSE)</f>
+        <v/>
+      </c>
+      <c r="B134" s="0" t="str">
+        <v>runyaover</v>
+      </c>
+      <c r="C134" s="0">
+        <v>39811802</v>
+      </c>
+      <c r="D134" s="12">
+        <v>45584.0</v>
+      </c>
+      <c r="E134" s="0">
+        <f>A134 &amp; "|" &amp; VLOOKUP(D134,SupportLists!D:E,2,FALSE)</f>
+        <v/>
+      </c>
+    </row>
+    <row r="135" spans="1:5" customFormat="false">
+      <c r="A135" s="0">
+        <f>VLOOKUP(B135,IDs!B:C,2,FALSE)</f>
+        <v/>
+      </c>
+      <c r="B135" s="0" t="str">
+        <v>Luna_Lulu</v>
+      </c>
+      <c r="C135" s="0">
+        <v>39057432</v>
+      </c>
+      <c r="D135" s="12">
+        <v>45584.0</v>
+      </c>
+      <c r="E135" s="0">
+        <f>A135 &amp; "|" &amp; VLOOKUP(D135,SupportLists!D:E,2,FALSE)</f>
+        <v/>
+      </c>
+    </row>
+    <row r="136" spans="1:5" customFormat="false">
+      <c r="A136" s="0">
+        <f>VLOOKUP(B136,IDs!B:C,2,FALSE)</f>
+        <v/>
+      </c>
+      <c r="B136" s="0" t="str">
+        <v>Lililulu</v>
+      </c>
+      <c r="C136" s="0">
+        <v>384728894</v>
+      </c>
+      <c r="D136" s="12">
+        <v>45584.0</v>
+      </c>
+      <c r="E136" s="0">
+        <f>A136 &amp; "|" &amp; VLOOKUP(D136,SupportLists!D:E,2,FALSE)</f>
+        <v/>
+      </c>
+    </row>
+    <row r="137" spans="1:5" customFormat="false">
+      <c r="A137" s="0">
+        <f>VLOOKUP(B137,IDs!B:C,2,FALSE)</f>
+        <v/>
+      </c>
+      <c r="B137" s="0" t="str">
+        <v>OldManLogan</v>
+      </c>
+      <c r="C137" s="0">
+        <v>37911832</v>
+      </c>
+      <c r="D137" s="12">
+        <v>45584.0</v>
+      </c>
+      <c r="E137" s="0">
+        <f>A137 &amp; "|" &amp; VLOOKUP(D137,SupportLists!D:E,2,FALSE)</f>
+        <v/>
+      </c>
+    </row>
+    <row r="138" spans="1:5" customFormat="false">
+      <c r="A138" s="0">
+        <f>VLOOKUP(B138,IDs!B:C,2,FALSE)</f>
+        <v/>
+      </c>
+      <c r="B138" s="0" t="str">
+        <v>VonTempsky</v>
+      </c>
+      <c r="C138" s="0">
+        <v>37176660</v>
+      </c>
+      <c r="D138" s="12">
+        <v>45584.0</v>
+      </c>
+      <c r="E138" s="0">
+        <f>A138 &amp; "|" &amp; VLOOKUP(D138,SupportLists!D:E,2,FALSE)</f>
+        <v/>
+      </c>
+    </row>
+    <row r="139" spans="1:5" customFormat="false">
+      <c r="A139" s="0">
+        <f>VLOOKUP(B139,IDs!B:C,2,FALSE)</f>
+        <v/>
+      </c>
+      <c r="B139" s="0" t="str">
+        <v>Odin1206</v>
+      </c>
+      <c r="C139" s="0">
+        <v>36118388</v>
+      </c>
+      <c r="D139" s="12">
+        <v>45584.0</v>
+      </c>
+      <c r="E139" s="0">
+        <f>A139 &amp; "|" &amp; VLOOKUP(D139,SupportLists!D:E,2,FALSE)</f>
+        <v/>
+      </c>
+    </row>
+    <row r="140" spans="1:5" customFormat="false">
+      <c r="A140" s="0">
+        <f>VLOOKUP(B140,IDs!B:C,2,FALSE)</f>
+        <v/>
+      </c>
+      <c r="B140" s="0" t="str">
+        <v>MizzBond</v>
+      </c>
+      <c r="C140" s="0">
+        <v>35423556</v>
+      </c>
+      <c r="D140" s="12">
+        <v>45584.0</v>
+      </c>
+      <c r="E140" s="0">
+        <f>A140 &amp; "|" &amp; VLOOKUP(D140,SupportLists!D:E,2,FALSE)</f>
+        <v/>
+      </c>
+    </row>
+    <row r="141" spans="1:5" customFormat="false">
+      <c r="A141" s="0">
+        <f>VLOOKUP(B141,IDs!B:C,2,FALSE)</f>
+        <v/>
+      </c>
+      <c r="B141" s="0" t="str">
+        <v>Brilith</v>
+      </c>
+      <c r="C141" s="0">
+        <v>38241597</v>
+      </c>
+      <c r="D141" s="12">
+        <v>45584.0</v>
+      </c>
+      <c r="E141" s="0">
+        <f>A141 &amp; "|" &amp; VLOOKUP(D141,SupportLists!D:E,2,FALSE)</f>
+        <v/>
+      </c>
+    </row>
+    <row r="142" spans="1:5" customFormat="false">
+      <c r="A142" s="0">
+        <f>VLOOKUP(B142,IDs!B:C,2,FALSE)</f>
+        <v/>
+      </c>
+      <c r="B142" s="0" t="str">
+        <v>Elo785</v>
+      </c>
+      <c r="C142" s="0">
+        <v>37512673</v>
+      </c>
+      <c r="D142" s="12">
+        <v>45584.0</v>
+      </c>
+      <c r="E142" s="0">
+        <f>A142 &amp; "|" &amp; VLOOKUP(D142,SupportLists!D:E,2,FALSE)</f>
+        <v/>
+      </c>
+    </row>
+    <row r="143" spans="1:5" customFormat="false">
+      <c r="A143" s="0">
+        <f>VLOOKUP(B143,IDs!B:C,2,FALSE)</f>
+        <v/>
+      </c>
+      <c r="B143" s="0" t="str">
+        <v>Pilot_</v>
+      </c>
+      <c r="C143" s="0">
+        <v>36293400</v>
+      </c>
+      <c r="D143" s="12">
+        <v>45584.0</v>
+      </c>
+      <c r="E143" s="0">
+        <f>A143 &amp; "|" &amp; VLOOKUP(D143,SupportLists!D:E,2,FALSE)</f>
+        <v/>
+      </c>
+    </row>
+    <row r="144" spans="1:5" customFormat="false">
+      <c r="A144" s="0">
+        <f>VLOOKUP(B144,IDs!B:C,2,FALSE)</f>
+        <v/>
+      </c>
+      <c r="B144" s="0" t="str">
+        <v>Lucky6612</v>
+      </c>
+      <c r="C144" s="0">
+        <v>35810392</v>
+      </c>
+      <c r="D144" s="12">
+        <v>45584.0</v>
+      </c>
+      <c r="E144" s="0">
+        <f>A144 &amp; "|" &amp; VLOOKUP(D144,SupportLists!D:E,2,FALSE)</f>
+        <v/>
+      </c>
+    </row>
+    <row r="145" spans="1:5" customFormat="false">
+      <c r="A145" s="0">
+        <f>VLOOKUP(B145,IDs!B:C,2,FALSE)</f>
+        <v/>
+      </c>
+      <c r="B145" s="0" t="str">
+        <v>Omilixo</v>
+      </c>
+      <c r="C145" s="0">
+        <v>34953211</v>
+      </c>
+      <c r="D145" s="12">
+        <v>45584.0</v>
+      </c>
+      <c r="E145" s="0">
+        <f>A145 &amp; "|" &amp; VLOOKUP(D145,SupportLists!D:E,2,FALSE)</f>
+        <v/>
+      </c>
+    </row>
+    <row r="146" spans="1:5" customFormat="false">
+      <c r="A146" s="0">
+        <f>VLOOKUP(B146,IDs!B:C,2,FALSE)</f>
+        <v/>
+      </c>
+      <c r="B146" s="0" t="str">
+        <v>chenjun</v>
+      </c>
+      <c r="C146" s="0">
+        <v>33548915</v>
+      </c>
+      <c r="D146" s="12">
+        <v>45584.0</v>
+      </c>
+      <c r="E146" s="0">
+        <f>A146 &amp; "|" &amp; VLOOKUP(D146,SupportLists!D:E,2,FALSE)</f>
+        <v/>
+      </c>
+    </row>
+    <row r="147" spans="1:5" customFormat="false">
+      <c r="A147" s="0">
+        <f>VLOOKUP(B147,IDs!B:C,2,FALSE)</f>
+        <v/>
+      </c>
+      <c r="B147" s="0" t="str">
+        <v>Fab1250</v>
+      </c>
+      <c r="C147" s="0">
+        <v>34546068</v>
+      </c>
+      <c r="D147" s="12">
+        <v>45584.0</v>
+      </c>
+      <c r="E147" s="0">
+        <f>A147 &amp; "|" &amp; VLOOKUP(D147,SupportLists!D:E,2,FALSE)</f>
+        <v/>
+      </c>
+    </row>
+    <row r="148" spans="1:5" customFormat="false">
+      <c r="A148" s="0">
+        <f>VLOOKUP(B148,IDs!B:C,2,FALSE)</f>
+        <v/>
+      </c>
+      <c r="B148" s="0" t="str">
+        <v>Valessa</v>
+      </c>
+      <c r="C148" s="0">
+        <v>56755772</v>
+      </c>
+      <c r="D148" s="12">
+        <v>45584.0</v>
+      </c>
+      <c r="E148" s="0">
+        <f>A148 &amp; "|" &amp; VLOOKUP(D148,SupportLists!D:E,2,FALSE)</f>
+        <v/>
+      </c>
+    </row>
+    <row r="149" spans="1:5" customFormat="false">
+      <c r="A149" s="0">
+        <f>VLOOKUP(B149,IDs!B:C,2,FALSE)</f>
+        <v/>
+      </c>
+      <c r="B149" s="0" t="str">
+        <v>BasilFawlty</v>
+      </c>
+      <c r="C149" s="0">
+        <v>75666591</v>
+      </c>
+      <c r="D149" s="12">
+        <v>45584.0</v>
+      </c>
+      <c r="E149" s="0">
+        <f>A149 &amp; "|" &amp; VLOOKUP(D149,SupportLists!D:E,2,FALSE)</f>
+        <v/>
+      </c>
+    </row>
+    <row r="150" spans="1:5" customFormat="false">
+      <c r="A150" s="0">
+        <f>VLOOKUP(B150,IDs!B:C,2,FALSE)</f>
+        <v/>
+      </c>
+      <c r="B150" s="0" t="str">
+        <v>LewkSkywatcher</v>
+      </c>
+      <c r="C150" s="0">
+        <v>53752299</v>
+      </c>
+      <c r="D150" s="12">
+        <v>45584.0</v>
+      </c>
+      <c r="E150" s="0">
+        <f>A150 &amp; "|" &amp; VLOOKUP(D150,SupportLists!D:E,2,FALSE)</f>
+        <v/>
+      </c>
+    </row>
+    <row r="151" spans="1:5" customFormat="false">
+      <c r="A151" s="0">
+        <f>VLOOKUP(B151,IDs!B:C,2,FALSE)</f>
+        <v/>
+      </c>
+      <c r="B151" s="0" t="str">
+        <v>ocdMonkey</v>
+      </c>
+      <c r="C151" s="0">
+        <v>54250384</v>
+      </c>
+      <c r="D151" s="12">
+        <v>45584.0</v>
+      </c>
+      <c r="E151" s="0">
+        <f>A151 &amp; "|" &amp; VLOOKUP(D151,SupportLists!D:E,2,FALSE)</f>
+        <v/>
+      </c>
+    </row>
+    <row r="152" spans="1:5" customFormat="false">
+      <c r="A152" s="0">
+        <f>VLOOKUP(B152,IDs!B:C,2,FALSE)</f>
+        <v/>
+      </c>
+      <c r="B152" s="0" t="str">
+        <v>DropKick4</v>
+      </c>
+      <c r="C152" s="0">
+        <v>48578895</v>
+      </c>
+      <c r="D152" s="12">
+        <v>45584.0</v>
+      </c>
+      <c r="E152" s="0">
+        <f>A152 &amp; "|" &amp; VLOOKUP(D152,SupportLists!D:E,2,FALSE)</f>
+        <v/>
+      </c>
+    </row>
+    <row r="153" spans="1:5" customFormat="false">
+      <c r="A153" s="0">
+        <f>VLOOKUP(B153,IDs!B:C,2,FALSE)</f>
+        <v/>
+      </c>
+      <c r="B153" s="0" t="str">
+        <v>CMLTO</v>
+      </c>
+      <c r="C153" s="0">
+        <v>66778954</v>
+      </c>
+      <c r="D153" s="12">
+        <v>45584.0</v>
+      </c>
+      <c r="E153" s="0">
+        <f>A153 &amp; "|" &amp; VLOOKUP(D153,SupportLists!D:E,2,FALSE)</f>
+        <v/>
+      </c>
+    </row>
+    <row r="154" spans="1:5" customFormat="false">
+      <c r="A154" s="0">
+        <f>VLOOKUP(B154,IDs!B:C,2,FALSE)</f>
+        <v/>
+      </c>
+      <c r="B154" s="0" t="str">
+        <v>WhoDey812</v>
+      </c>
+      <c r="C154" s="0">
+        <v>59781609</v>
+      </c>
+      <c r="D154" s="12">
+        <v>45584.0</v>
+      </c>
+      <c r="E154" s="0">
+        <f>A154 &amp; "|" &amp; VLOOKUP(D154,SupportLists!D:E,2,FALSE)</f>
+        <v/>
+      </c>
+    </row>
+    <row r="155" spans="1:5" customFormat="false">
+      <c r="A155" s="0">
+        <f>VLOOKUP(B155,IDs!B:C,2,FALSE)</f>
+        <v/>
+      </c>
+      <c r="B155" s="0" t="str">
+        <v>Horizen</v>
+      </c>
+      <c r="C155" s="0">
+        <v>60231598</v>
+      </c>
+      <c r="D155" s="12">
+        <v>45584.0</v>
+      </c>
+      <c r="E155" s="0">
+        <f>A155 &amp; "|" &amp; VLOOKUP(D155,SupportLists!D:E,2,FALSE)</f>
+        <v/>
+      </c>
+    </row>
+    <row r="156" spans="1:5" customFormat="false">
+      <c r="A156" s="0">
+        <f>VLOOKUP(B156,IDs!B:C,2,FALSE)</f>
+        <v/>
+      </c>
+      <c r="B156" s="0" t="str">
+        <v>Amcoone</v>
+      </c>
+      <c r="C156" s="0">
+        <v>417634243</v>
+      </c>
+      <c r="D156" s="12">
+        <v>45584.0</v>
+      </c>
+      <c r="E156" s="0">
+        <f>A156 &amp; "|" &amp; VLOOKUP(D156,SupportLists!D:E,2,FALSE)</f>
+        <v/>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
sync print and excel output
</commit_message>
<xml_diff>
--- a/new.xlsx
+++ b/new.xlsx
@@ -7062,7 +7062,7 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3">
-  <dimension ref="A1:D1"/>
+  <dimension ref="A1:I10"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="O7" sqref="O7"/>
@@ -7084,6 +7084,285 @@
         <v>3</v>
       </c>
     </row>
+    <row r="2" spans="1:9" customFormat="false">
+      <c r="A2" s="0">
+        <f>VLOOKUP(B2,IDs!B:C,2,FALSE)</f>
+        <v/>
+      </c>
+      <c r="B2" s="0" t="str">
+        <v>Nyarlathotep</v>
+      </c>
+      <c r="C2" s="0">
+        <v>614</v>
+      </c>
+      <c r="D2" s="0">
+        <v>2</v>
+      </c>
+      <c r="E2" s="0" t="str">
+        <v>Yamagata</v>
+      </c>
+      <c r="F2" s="0" t="str">
+        <v>dm</v>
+      </c>
+      <c r="G2" s="0" t="str">
+        <v>dm</v>
+      </c>
+      <c r="H2" s="12">
+        <v>45584.0</v>
+      </c>
+      <c r="I2" s="0">
+        <f>TODAY()-G2</f>
+        <v/>
+      </c>
+    </row>
+    <row r="3" spans="1:9" customFormat="false">
+      <c r="A3" s="0">
+        <f>VLOOKUP(B3,IDs!B:C,2,FALSE)</f>
+        <v/>
+      </c>
+      <c r="B3" s="0" t="str">
+        <v>Alecks_</v>
+      </c>
+      <c r="C3" s="0">
+        <v>334</v>
+      </c>
+      <c r="D3" s="0">
+        <v>2</v>
+      </c>
+      <c r="E3" s="0" t="str">
+        <v>Yamagata</v>
+      </c>
+      <c r="F3" s="0" t="str">
+        <v>dm</v>
+      </c>
+      <c r="G3" s="0" t="str">
+        <v>dm</v>
+      </c>
+      <c r="H3" s="12">
+        <v>45584.0</v>
+      </c>
+      <c r="I3" s="0">
+        <f>TODAY()-G3</f>
+        <v/>
+      </c>
+    </row>
+    <row r="4" spans="1:9" customFormat="false">
+      <c r="A4" s="0">
+        <f>VLOOKUP(B4,IDs!B:C,2,FALSE)</f>
+        <v/>
+      </c>
+      <c r="B4" s="0" t="str">
+        <v>Noah</v>
+      </c>
+      <c r="C4" s="0">
+        <v>311</v>
+      </c>
+      <c r="D4" s="0">
+        <v>2</v>
+      </c>
+      <c r="E4" s="0" t="str">
+        <v>Yamagata</v>
+      </c>
+      <c r="F4" s="0" t="str">
+        <v>dm</v>
+      </c>
+      <c r="G4" s="0" t="str">
+        <v>dm</v>
+      </c>
+      <c r="H4" s="12">
+        <v>45584.0</v>
+      </c>
+      <c r="I4" s="0">
+        <f>TODAY()-G4</f>
+        <v/>
+      </c>
+    </row>
+    <row r="5" spans="1:9" customFormat="false">
+      <c r="A5" s="0">
+        <f>VLOOKUP(B5,IDs!B:C,2,FALSE)</f>
+        <v/>
+      </c>
+      <c r="B5" s="0" t="str">
+        <v>Aileen</v>
+      </c>
+      <c r="C5" s="0">
+        <v>254</v>
+      </c>
+      <c r="D5" s="0">
+        <v>2</v>
+      </c>
+      <c r="E5" s="0" t="str">
+        <v>Yamagata</v>
+      </c>
+      <c r="F5" s="0" t="str">
+        <v>dm</v>
+      </c>
+      <c r="G5" s="0" t="str">
+        <v>dm</v>
+      </c>
+      <c r="H5" s="12">
+        <v>45584.0</v>
+      </c>
+      <c r="I5" s="0">
+        <f>TODAY()-G5</f>
+        <v/>
+      </c>
+    </row>
+    <row r="6" spans="1:9" customFormat="false">
+      <c r="A6" s="0">
+        <f>VLOOKUP(B6,IDs!B:C,2,FALSE)</f>
+        <v/>
+      </c>
+      <c r="B6" s="0" t="str">
+        <v>Letsi</v>
+      </c>
+      <c r="C6" s="0">
+        <v>240</v>
+      </c>
+      <c r="D6" s="0">
+        <v>2</v>
+      </c>
+      <c r="E6" s="0" t="str">
+        <v>Yamagata</v>
+      </c>
+      <c r="F6" s="0" t="str">
+        <v>dm</v>
+      </c>
+      <c r="G6" s="0" t="str">
+        <v>dm</v>
+      </c>
+      <c r="H6" s="12">
+        <v>45584.0</v>
+      </c>
+      <c r="I6" s="0">
+        <f>TODAY()-G6</f>
+        <v/>
+      </c>
+    </row>
+    <row r="7" spans="1:9" customFormat="false">
+      <c r="A7" s="0">
+        <f>VLOOKUP(B7,IDs!B:C,2,FALSE)</f>
+        <v/>
+      </c>
+      <c r="B7" s="0" t="str">
+        <v>Nefi85</v>
+      </c>
+      <c r="C7" s="0">
+        <v>70</v>
+      </c>
+      <c r="D7" s="0">
+        <v>2</v>
+      </c>
+      <c r="E7" s="0" t="str">
+        <v>Yamagata</v>
+      </c>
+      <c r="F7" s="0" t="str">
+        <v>dm</v>
+      </c>
+      <c r="G7" s="0" t="str">
+        <v>dm</v>
+      </c>
+      <c r="H7" s="12">
+        <v>45584.0</v>
+      </c>
+      <c r="I7" s="0">
+        <f>TODAY()-G7</f>
+        <v/>
+      </c>
+    </row>
+    <row r="8" spans="1:9" customFormat="false">
+      <c r="A8" s="0">
+        <f>VLOOKUP(B8,IDs!B:C,2,FALSE)</f>
+        <v/>
+      </c>
+      <c r="B8" s="0" t="str">
+        <v>xljhx31</v>
+      </c>
+      <c r="C8" s="0">
+        <v>58</v>
+      </c>
+      <c r="D8" s="0">
+        <v>2</v>
+      </c>
+      <c r="E8" s="0" t="str">
+        <v>Yamagata</v>
+      </c>
+      <c r="F8" s="0" t="str">
+        <v>dm</v>
+      </c>
+      <c r="G8" s="0" t="str">
+        <v>dm</v>
+      </c>
+      <c r="H8" s="12">
+        <v>45584.0</v>
+      </c>
+      <c r="I8" s="0">
+        <f>TODAY()-G8</f>
+        <v/>
+      </c>
+    </row>
+    <row r="9" spans="1:9" customFormat="false">
+      <c r="A9" s="0">
+        <f>VLOOKUP(B9,IDs!B:C,2,FALSE)</f>
+        <v/>
+      </c>
+      <c r="B9" s="0" t="str">
+        <v>mido009</v>
+      </c>
+      <c r="C9" s="0">
+        <v>55</v>
+      </c>
+      <c r="D9" s="0">
+        <v>2</v>
+      </c>
+      <c r="E9" s="0" t="str">
+        <v>Yamagata</v>
+      </c>
+      <c r="F9" s="0" t="str">
+        <v>dm</v>
+      </c>
+      <c r="G9" s="0" t="str">
+        <v>dm</v>
+      </c>
+      <c r="H9" s="12">
+        <v>45584.0</v>
+      </c>
+      <c r="I9" s="0">
+        <f>TODAY()-G9</f>
+        <v/>
+      </c>
+    </row>
+    <row r="10" spans="1:9" customFormat="false">
+      <c r="A10" s="0">
+        <f>VLOOKUP(B10,IDs!B:C,2,FALSE)</f>
+        <v/>
+      </c>
+      <c r="B10" s="0" t="str">
+        <v>Hallen98</v>
+      </c>
+      <c r="C10" s="0">
+        <v>44</v>
+      </c>
+      <c r="D10" s="0">
+        <v>2</v>
+      </c>
+      <c r="E10" s="0" t="str">
+        <v>Yamagata</v>
+      </c>
+      <c r="F10" s="0" t="str">
+        <v>dm</v>
+      </c>
+      <c r="G10" s="0" t="str">
+        <v>dm</v>
+      </c>
+      <c r="H10" s="12">
+        <v>45584.0</v>
+      </c>
+      <c r="I10" s="0">
+        <f>TODAY()-G10</f>
+        <v/>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -7091,7 +7370,7 @@
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3">
-  <dimension ref="A1:F8"/>
+  <dimension ref="A1:F4"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="C3" sqref="C3"/>
@@ -7186,82 +7465,6 @@
       <c r="F4" t="e">
         <f t="shared" si="0"/>
         <v>#N/A</v>
-      </c>
-    </row>
-    <row r="5" spans="1:5" customFormat="false">
-      <c r="A5" s="0">
-        <f>VLOOKUP(B5,IDs!B:C,2,FALSE)</f>
-        <v/>
-      </c>
-      <c r="B5" s="0" t="str">
-        <v>Daeloan</v>
-      </c>
-      <c r="C5" s="0">
-        <v>14845250</v>
-      </c>
-      <c r="D5" s="12">
-        <v>45584.0</v>
-      </c>
-      <c r="E5" s="0">
-        <f>A5 &amp; "|" &amp; VLOOKUP(D5,SupportLists!D:E,2,FALSE)</f>
-        <v/>
-      </c>
-    </row>
-    <row r="6" spans="1:5" customFormat="false">
-      <c r="A6" s="0">
-        <f>VLOOKUP(B6,IDs!B:C,2,FALSE)</f>
-        <v/>
-      </c>
-      <c r="B6" s="0" t="str">
-        <v>kafka</v>
-      </c>
-      <c r="C6" s="0">
-        <v>9422204</v>
-      </c>
-      <c r="D6" s="12">
-        <v>45584.0</v>
-      </c>
-      <c r="E6" s="0">
-        <f>A6 &amp; "|" &amp; VLOOKUP(D6,SupportLists!D:E,2,FALSE)</f>
-        <v/>
-      </c>
-    </row>
-    <row r="7" spans="1:5" customFormat="false">
-      <c r="A7" s="0">
-        <f>VLOOKUP(B7,IDs!B:C,2,FALSE)</f>
-        <v/>
-      </c>
-      <c r="B7" s="0" t="str">
-        <v>Brilith</v>
-      </c>
-      <c r="C7" s="0">
-        <v>5800627</v>
-      </c>
-      <c r="D7" s="12">
-        <v>45584.0</v>
-      </c>
-      <c r="E7" s="0">
-        <f>A7 &amp; "|" &amp; VLOOKUP(D7,SupportLists!D:E,2,FALSE)</f>
-        <v/>
-      </c>
-    </row>
-    <row r="8" spans="1:5" customFormat="false">
-      <c r="A8" s="0">
-        <f>VLOOKUP(B8,IDs!B:C,2,FALSE)</f>
-        <v/>
-      </c>
-      <c r="B8" s="0" t="str">
-        <v>Mr.Skieyagi69</v>
-      </c>
-      <c r="C8" s="0">
-        <v>4021875</v>
-      </c>
-      <c r="D8" s="12">
-        <v>45584.0</v>
-      </c>
-      <c r="E8" s="0">
-        <f>A8 &amp; "|" &amp; VLOOKUP(D8,SupportLists!D:E,2,FALSE)</f>
-        <v/>
       </c>
     </row>
   </sheetData>

</xml_diff>